<commit_message>
Ran Ethiopia process with updated parameter files
From Wudu: updated cattle subnational parameters
From Andrew: updated small ruminant disease-specific parameters
10 simulation runs of AHLE function
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/Code and Control Files/Subnational parameters/Afar 2021_AHLE scenario parameters CATTLE scenarios only.xlsx
+++ b/Ethiopia Workspace/Code and Control Files/Subnational parameters/Afar 2021_AHLE scenario parameters CATTLE scenarios only.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\First Analytics\Clients\University of Liverpool\GBADs Github\GBADsLiverpool\Ethiopia Workspace\Code and Control Files\AHLE parameter tables for subnational divisions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\First Analytics\Clients\University of Liverpool\GBADs Github\GBADsLiverpool\Ethiopia Workspace\Code and Control Files\Subnational parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDF698A-582D-4E90-9665-7CE3B2058964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AD9AC1-CDCD-478C-AFDD-36209F3BA2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="14292" windowWidth="23256" windowHeight="12720" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{7B09E95E-6D5F-461A-A5DC-5B71F2D22658}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1650,20 +1650,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDE79AB-593E-49D8-BC0E-644D5608E970}">
   <dimension ref="A1:AV159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="O64" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="9" topLeftCell="C60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="R1" sqref="R1:R1048576"/>
+      <selection pane="bottomRight" activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="39.140625" style="28" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" style="28" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="28" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" style="28" customWidth="1"/>
     <col min="6" max="16" width="19.42578125" style="28" customWidth="1"/>
     <col min="17" max="17" width="19" style="28" customWidth="1"/>
     <col min="18" max="22" width="42.140625" bestFit="1" customWidth="1"/>
@@ -8035,46 +8035,46 @@
         <v>1</v>
       </c>
       <c r="D137" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E137" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F137" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G137" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H137" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I137" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J137" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K137" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L137" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M137" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N137" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O137" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P137" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q137" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R137" s="4"/>
       <c r="S137" s="4"/>

</xml_diff>